<commit_message>
Finish protege import rules
</commit_message>
<xml_diff>
--- a/protege/data/goodreads.xlsx
+++ b/protege/data/goodreads.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="194">
   <si>
     <t>authors</t>
   </si>
@@ -237,6 +237,18 @@
   </si>
   <si>
     <t>2016-03-28</t>
+  </si>
+  <si>
+    <t>Loved this! Was like nothing I'd ever read before, I couldn't put it down. I really connected with characters and got emotionally invested, also got my other half and my friends into the books!</t>
+  </si>
+  <si>
+    <t>2017-03-18</t>
+  </si>
+  <si>
+    <t>The first book of the Hunger Games trilogy.</t>
+  </si>
+  <si>
+    <t>2017-05-23</t>
   </si>
   <si>
     <t>My review on thinking for a while is different from the review that I would leave right after reading the book. When I got the book, it was a quick read and I was enthralled at the angsty and stressful story. But after thinking about it awhile, the story is more creepy and whiny than good. I was entertained though!</t>
@@ -291,6 +303,21 @@
     <t>2017-01-06</t>
   </si>
   <si>
+    <t>I have tried for years to shake my affection for Twilight. Self-sacrificing girl moves to the middle of nowhere. Girl meets boy. Boy barely manages to avoid eating girl. Boy and girl fall in love with each other. Boy stalks girl. Girl's okay with that. Boy probably won't kill girl, but he's making no promises. It's got a lot I like in a book passionate, chaste love-triangle-free romance (for the most part, if you stick to the first book); fantasy with a new perspective; excitement; a lot of pages. It's also repetitive, problematic, badly written. I was pretty surprised to see that I for the first time I couldn't enjoy it as much as before. Largely because for the first time, I read Edward as having no redeeming qualities. 
+ Edward Cullen is cold. I'm not talking about his stone lips. I never realized before how mean and uncaring he is. Anytime Bella is uncomfortable or unhappy, he's laughing at her. Intellectually, I knew that the Edward/Bella relationship is abusive and controlling. But I didn't realize how much Edward uses that awful put-the-girl-down-to-make-her-like-you technique. Ugh. Edward Cullen is definitely not what Twilight has going for it. 
+ Here's where Twilight's strengths are: The romantic/sexual tension in this book is largely very good. While I didn't find the meadow scene particularly compelling this go around, the build up to the first kiss is excellent. 
+ The book really feels like two different books. The first chapter through the baseball scene, plus the epilogue feel like one book, while the prologue and baseball scene to the last chapter has a totally different tone. While somewhat suspenseful, the first portion is a meandering romance, while the latter portion feels like a somewhat dull thriller. 
+ Overall, I wouldn't stop recommending this to fans of romance who can handle cheese. Although a handout identifying warning signs of abusive relationships nearby on the shelf wouldn't be a bad idea. I'm sure it's not my last reread, either. 
+ Why people turn on Twilight: 
+ -embarrassment because/ feeling of betrayal that they had liked Edward 
+ -Breaking Dawn There are so many things embarrassingly much worse about that book compared to the rest of the series. It breaks all the rules of the world that have been set up previously. Everything about Renesmee from her name to existence is ridiculous. And things with Jacob get very squicky. 
+ -because it inspires feverous praise, and then later people are embarrassed they praised it so much when they realize how flawed its writing/romance is 
+ -because it's just plain kind of embarrassingly cheesy</t>
+  </si>
+  <si>
+    <t>2017-02-07</t>
+  </si>
+  <si>
     <t>Whoa. Its different from the way I remember the movie. The movie works as a movie, but the book sure works well as a book. The movie builds to a dramatic ending, but the book keeps you on the edge throughout, and has charming moments to boot. I can't get enough of the lawyer as hero! Well worth the read.</t>
   </si>
   <si>
@@ -324,6 +351,14 @@
   </si>
   <si>
     <t>2016-01-17</t>
+  </si>
+  <si>
+    <t>I really should become more acquainted with the classic works of fiction and this is one, albeit from the 60s rather than the 19th Century, but still. As hard as it may be to fathom this, I didn't know anything about the novel other than its Great Depression, Deep South setting. It is certainly eye opening today to hear the liberal use of racial epithets (the N word most notably) although it is certainly in keeping with the times and the location. 
+ As much as I am fighting against it, I am a literary philistine when it comes to classic fiction. I spend most of my leisure reading time on non-fiction of all types so my reviews and ratings are often filtered through that lens. I very much enjoyed this novel, speaking as it does to the vile force that was and is racism in this country. Atticus Finch is certainly a worthy hero and I can see why this book is often taught in schools, despite the racism that is front and center. Atticus' attitude and belief system is admirable and his integrity shines through the whole narrative. His is certainly an attitude to life worth emulating. 
+ The plot is not complex, taking place over three years but the racial themes, the loss of innocence, the lack of real justice and the humanity that runs through the narrator's father certainly make it pretty gripping reading. I am glad I read it and feel better informed, in my own small way, on a subject that is viscerally important to my liberal, bleeding heart!</t>
+  </si>
+  <si>
+    <t>2017-10-01</t>
   </si>
   <si>
     <t>** spoiler alert ** 
@@ -424,6 +459,12 @@
   </si>
   <si>
     <t>2016-02-04</t>
+  </si>
+  <si>
+    <t>Tried reading this years ago and couldn't deal with the slow pace; this time I listened to an audiobook version and loved it!</t>
+  </si>
+  <si>
+    <t>2016-09-23</t>
   </si>
   <si>
     <t>I love this book. It is well-written and intriguing. I won't include any spoilers. I will say that you are missing so much of the story if you only see the movie. Now I need to get a copy of Insurgent!</t>
@@ -626,6 +667,13 @@
   </si>
   <si>
     <t>2017-02-12</t>
+  </si>
+  <si>
+    <t>qm@ lmd@ 6 'ym fy `lm slsl@ rwyt ljw` .. lm ynqT` l fy lmHDrt wlskshn D .. bs ll'sf nthyt mnh bnfs Hl@ ly's lty nthy bh mn kl rwy@ ydf`ny HZy l`thr lqry'th mw'khr .. klh m'swy@ :/ 
+ wd` Hzyn lrwy@ ry'`@ .. shkr</t>
+  </si>
+  <si>
+    <t>2016-02-10</t>
   </si>
 </sst>
 </file>
@@ -895,7 +943,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="14.57"/>
     <col customWidth="1" min="2" max="2" width="9.29"/>
@@ -2169,7 +2217,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="14.57"/>
     <col customWidth="1" min="2" max="2" width="13.43"/>
@@ -3340,1192 +3388,1514 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.29"/>
-    <col customWidth="1" min="2" max="2" width="52.14"/>
-    <col customWidth="1" min="3" max="3" width="12.14"/>
-    <col customWidth="1" min="4" max="4" width="119.57"/>
-    <col customWidth="1" min="5" max="5" width="10.43"/>
-    <col customWidth="1" min="6" max="26" width="11.57"/>
+    <col customWidth="1" min="1" max="1" width="7.29"/>
+    <col customWidth="1" min="2" max="2" width="9.29"/>
+    <col customWidth="1" min="3" max="3" width="52.14"/>
+    <col customWidth="1" min="4" max="4" width="12.14"/>
+    <col customWidth="1" min="5" max="5" width="86.0"/>
+    <col customWidth="1" min="6" max="6" width="10.43"/>
+    <col customWidth="1" min="7" max="26" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="1">
+        <v>461149.0</v>
+      </c>
+      <c r="B2" s="1">
         <v>2767052.0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>3.0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="1">
+        <v>462390.0</v>
+      </c>
+      <c r="B3" s="1">
         <v>2767052.0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>3.0</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="1">
+        <v>462603.0</v>
+      </c>
+      <c r="B4" s="1">
         <v>2767052.0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>4.0</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="1">
+        <v>462744.0</v>
+      </c>
+      <c r="B5" s="1">
         <v>2767052.0</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>5.0</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="1">
+        <v>462749.0</v>
+      </c>
+      <c r="B6" s="1">
         <v>2767052.0</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>5.0</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="1">
+        <v>463375.0</v>
+      </c>
+      <c r="B7" s="1">
         <v>2767052.0</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>4.0</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="1">
-        <v>41865.0</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D8" s="1" t="s">
+        <v>463982.0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2767052.0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="1">
-        <v>41865.0</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1">
+        <v>464001.0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2767052.0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1">
         <v>3.0</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="1">
+        <v>57010.0</v>
+      </c>
+      <c r="B10" s="1">
         <v>41865.0</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="1">
+        <v>57763.0</v>
+      </c>
+      <c r="B11" s="1">
         <v>41865.0</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="1">
+        <v>58477.0</v>
+      </c>
+      <c r="B12" s="1">
         <v>41865.0</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>3.0</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="1">
+        <v>58755.0</v>
+      </c>
+      <c r="B13" s="1">
         <v>41865.0</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="1">
+        <v>60253.0</v>
+      </c>
+      <c r="B14" s="1">
         <v>41865.0</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="1">
-        <v>2657.0</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D15" s="1" t="s">
+        <v>62423.0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>41865.0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="1">
-        <v>2657.0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D16" s="3" t="s">
+        <v>62922.0</v>
+      </c>
+      <c r="B16" s="1">
+        <v>41865.0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="1">
-        <v>2657.0</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D17" s="1" t="s">
+        <v>63537.0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>41865.0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="1">
+        <v>131287.0</v>
+      </c>
+      <c r="B18" s="1">
         <v>2657.0</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>90</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="1">
+        <v>131381.0</v>
+      </c>
+      <c r="B19" s="1">
         <v>2657.0</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <v>5.0</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="3" t="s">
         <v>92</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="1">
+        <v>131587.0</v>
+      </c>
+      <c r="B20" s="1">
         <v>2657.0</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>5.0</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>94</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="1">
-        <v>960.0</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="1">
+        <v>131727.0</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2657.0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="1">
         <v>5.0</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="1">
-        <v>960.0</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D22" s="1" t="s">
+        <v>131941.0</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2657.0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="1">
-        <v>960.0</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="1">
+        <v>132319.0</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2657.0</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="1">
         <v>5.0</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="1">
-        <v>960.0</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D24" s="1" t="s">
+        <v>132341.0</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2657.0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="1">
+        <v>241941.0</v>
+      </c>
+      <c r="B25" s="1">
         <v>960.0</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="1">
+        <v>242632.0</v>
+      </c>
+      <c r="B26" s="1">
         <v>960.0</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="1">
+        <v>242881.0</v>
+      </c>
+      <c r="B27" s="1">
         <v>960.0</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="1">
+      <c r="D27" s="1">
         <v>5.0</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="1">
+        <v>243182.0</v>
+      </c>
+      <c r="B28" s="1">
         <v>960.0</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D28" s="1">
         <v>5.0</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="1">
-        <v>1885.0</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D29" s="1" t="s">
+        <v>245793.0</v>
+      </c>
+      <c r="B29" s="1">
+        <v>960.0</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>89</v>
+      <c r="F29" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="1">
-        <v>1885.0</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E30" s="2" t="s">
+        <v>246824.0</v>
+      </c>
+      <c r="B30" s="1">
+        <v>960.0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>113</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="1">
-        <v>1885.0</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="1">
+        <v>247102.0</v>
+      </c>
+      <c r="B31" s="1">
+        <v>960.0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1">
         <v>5.0</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="1" t="s">
         <v>115</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="1">
-        <v>1885.0</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E32" s="2" t="s">
+        <v>247273.0</v>
+      </c>
+      <c r="B32" s="1">
+        <v>960.0</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>117</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="1">
+        <v>357473.0</v>
+      </c>
+      <c r="B33" s="1">
         <v>1885.0</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D33" s="1">
         <v>5.0</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="1" t="s">
         <v>119</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="1">
+        <v>357722.0</v>
+      </c>
+      <c r="B34" s="1">
         <v>1885.0</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="1">
+        <v>357953.0</v>
+      </c>
+      <c r="B35" s="1">
         <v>1885.0</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="1">
+      <c r="D35" s="1">
         <v>5.0</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="1">
-        <v>1.3335037E7</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D36" s="1" t="s">
+        <v>358277.0</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1885.0</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="1">
-        <v>1.3335037E7</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="1">
+        <v>358361.0</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1885.0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="1">
         <v>5.0</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>73</v>
+      <c r="F37" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="1">
-        <v>1.3335037E7</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E38" s="2" t="s">
+        <v>358367.0</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1885.0</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>128</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="1">
-        <v>1.3335037E7</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" s="1">
+        <v>358460.0</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1885.0</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="1">
         <v>5.0</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="3" t="s">
         <v>130</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="1">
-        <v>1.3335037E7</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E40" s="2" t="s">
+        <v>358546.0</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1885.0</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>132</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="1">
+        <v>461411.0</v>
+      </c>
+      <c r="B41" s="1">
         <v>1.3335037E7</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E41" s="2" t="s">
+      <c r="D41" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>134</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="42" ht="12.75" customHeight="1">
       <c r="A42" s="1">
+        <v>461454.0</v>
+      </c>
+      <c r="B42" s="1">
         <v>1.3335037E7</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E42" s="2" t="s">
+      <c r="D42" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>136</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="1">
+        <v>461953.0</v>
+      </c>
+      <c r="B43" s="1">
         <v>1.3335037E7</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="1">
-        <v>48855.0</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="1">
+        <v>462080.0</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1.3335037E7</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="1">
         <v>5.0</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>89</v>
+      <c r="F44" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="45" ht="12.75" customHeight="1">
       <c r="A45" s="1">
-        <v>48855.0</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E45" s="2" t="s">
+        <v>462667.0</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1.3335037E7</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>141</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="46" ht="12.75" customHeight="1">
       <c r="A46" s="1">
-        <v>48855.0</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" s="1">
+        <v>464372.0</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1.3335037E7</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="1">
         <v>4.0</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="3" t="s">
         <v>143</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" s="1">
-        <v>48855.0</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" s="1">
+        <v>464919.0</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1.3335037E7</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="1">
         <v>4.0</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="1" t="s">
         <v>145</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="48" ht="12.75" customHeight="1">
       <c r="A48" s="1">
-        <v>48855.0</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E48" s="2" t="s">
+        <v>464941.0</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1.3335037E7</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>147</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="49" ht="12.75" customHeight="1">
       <c r="A49" s="1">
+        <v>131581.0</v>
+      </c>
+      <c r="B49" s="1">
         <v>48855.0</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="1">
+      <c r="D49" s="1">
         <v>5.0</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="1" t="s">
         <v>149</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="50" ht="12.75" customHeight="1">
       <c r="A50" s="1">
+        <v>131936.0</v>
+      </c>
+      <c r="B50" s="1">
         <v>48855.0</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="51" ht="12.75" customHeight="1">
       <c r="A51" s="1">
-        <v>2429135.0</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C51" s="1">
+        <v>132247.0</v>
+      </c>
+      <c r="B51" s="1">
+        <v>48855.0</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="1">
         <v>4.0</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="52" ht="12.75" customHeight="1">
       <c r="A52" s="1">
-        <v>2429135.0</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D52" s="1" t="s">
+        <v>132299.0</v>
+      </c>
+      <c r="B52" s="1">
+        <v>48855.0</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>153</v>
+      <c r="F52" s="2" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="53" ht="12.75" customHeight="1">
       <c r="A53" s="1">
-        <v>2429135.0</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C53" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E53" s="2" t="s">
+        <v>132957.0</v>
+      </c>
+      <c r="B53" s="1">
+        <v>48855.0</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>156</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="54" ht="12.75" customHeight="1">
       <c r="A54" s="1">
-        <v>2429135.0</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E54" s="2" t="s">
+        <v>133754.0</v>
+      </c>
+      <c r="B54" s="1">
+        <v>48855.0</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>158</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="55" ht="12.75" customHeight="1">
       <c r="A55" s="1">
-        <v>2429135.0</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C55" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>92</v>
+        <v>133970.0</v>
+      </c>
+      <c r="B55" s="1">
+        <v>48855.0</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="56" ht="12.75" customHeight="1">
       <c r="A56" s="1">
+        <v>241637.0</v>
+      </c>
+      <c r="B56" s="1">
         <v>2429135.0</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C56" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>161</v>
+      <c r="D56" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="57" ht="12.75" customHeight="1">
       <c r="A57" s="1">
-        <v>6148028.0</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C57" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>61</v>
+        <v>242892.0</v>
+      </c>
+      <c r="B57" s="1">
+        <v>2429135.0</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="58" ht="12.75" customHeight="1">
       <c r="A58" s="1">
-        <v>6148028.0</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C58" s="1">
+        <v>243289.0</v>
+      </c>
+      <c r="B58" s="1">
+        <v>2429135.0</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" s="1">
         <v>4.0</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>153</v>
+      <c r="E58" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="59" ht="12.75" customHeight="1">
       <c r="A59" s="1">
-        <v>6148028.0</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C59" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>165</v>
+        <v>244642.0</v>
+      </c>
+      <c r="B59" s="1">
+        <v>2429135.0</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="60" ht="12.75" customHeight="1">
       <c r="A60" s="1">
-        <v>6148028.0</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" s="1">
+        <v>244779.0</v>
+      </c>
+      <c r="B60" s="1">
+        <v>2429135.0</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="1">
         <v>4.0</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>115</v>
+      <c r="E60" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="61" ht="12.75" customHeight="1">
       <c r="A61" s="1">
-        <v>6148028.0</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C61" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>168</v>
+        <v>244935.0</v>
+      </c>
+      <c r="B61" s="1">
+        <v>2429135.0</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="62" ht="12.75" customHeight="1">
       <c r="A62" s="1">
+        <v>462388.0</v>
+      </c>
+      <c r="B62" s="1">
         <v>6148028.0</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C62" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>170</v>
+      <c r="D62" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="63" ht="12.75" customHeight="1">
       <c r="A63" s="1">
-        <v>7260188.0</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C63" s="1">
+        <v>468367.0</v>
+      </c>
+      <c r="B63" s="1">
+        <v>6148028.0</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" s="1">
         <v>4.0</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>172</v>
+      <c r="E63" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="64" ht="12.75" customHeight="1">
       <c r="A64" s="1">
-        <v>7260188.0</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C64" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>65</v>
+        <v>468509.0</v>
+      </c>
+      <c r="B64" s="1">
+        <v>6148028.0</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="65" ht="12.75" customHeight="1">
       <c r="A65" s="1">
-        <v>7260188.0</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C65" s="1">
+        <v>468699.0</v>
+      </c>
+      <c r="B65" s="1">
+        <v>6148028.0</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D65" s="1">
         <v>4.0</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>61</v>
+      <c r="E65" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="66" ht="12.75" customHeight="1">
       <c r="A66" s="1">
-        <v>7260188.0</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C66" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>176</v>
+        <v>469573.0</v>
+      </c>
+      <c r="B66" s="1">
+        <v>6148028.0</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D66" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="67" ht="12.75" customHeight="1">
       <c r="A67" s="1">
-        <v>7260188.0</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C67" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>151</v>
+        <v>469711.0</v>
+      </c>
+      <c r="B67" s="1">
+        <v>6148028.0</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="68" ht="12.75" customHeight="1">
       <c r="A68" s="1">
+        <v>461291.0</v>
+      </c>
+      <c r="B68" s="1">
         <v>7260188.0</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C68" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>179</v>
+      <c r="D68" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="69" ht="12.75" customHeight="1">
       <c r="A69" s="1">
+        <v>461386.0</v>
+      </c>
+      <c r="B69" s="1">
         <v>7260188.0</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C69" s="1">
+      <c r="D69" s="1">
         <v>4.0</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="70" ht="12.75" customHeight="1"/>
-    <row r="71" ht="12.75" customHeight="1"/>
-    <row r="72" ht="12.75" customHeight="1"/>
-    <row r="73" ht="12.75" customHeight="1"/>
-    <row r="74" ht="12.75" customHeight="1"/>
-    <row r="75" ht="12.75" customHeight="1"/>
+      <c r="E69" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" ht="12.75" customHeight="1">
+      <c r="A70" s="1">
+        <v>462389.0</v>
+      </c>
+      <c r="B70" s="1">
+        <v>7260188.0</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D70" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" ht="12.75" customHeight="1">
+      <c r="A71" s="1">
+        <v>464196.0</v>
+      </c>
+      <c r="B71" s="1">
+        <v>7260188.0</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D71" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="72" ht="12.75" customHeight="1">
+      <c r="A72" s="1">
+        <v>466921.0</v>
+      </c>
+      <c r="B72" s="1">
+        <v>7260188.0</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D72" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="73" ht="12.75" customHeight="1">
+      <c r="A73" s="1">
+        <v>468366.0</v>
+      </c>
+      <c r="B73" s="1">
+        <v>7260188.0</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D73" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="74" ht="12.75" customHeight="1">
+      <c r="A74" s="1">
+        <v>468508.0</v>
+      </c>
+      <c r="B74" s="1">
+        <v>7260188.0</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" ht="12.75" customHeight="1">
+      <c r="A75" s="1">
+        <v>468591.0</v>
+      </c>
+      <c r="B75" s="1">
+        <v>7260188.0</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D75" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
     <row r="76" ht="12.75" customHeight="1"/>
     <row r="77" ht="12.75" customHeight="1"/>
     <row r="78" ht="12.75" customHeight="1"/>

</xml_diff>